<commit_message>
Kiwi pre tests data incorporated
</commit_message>
<xml_diff>
--- a/tape_test_xlsx.xlsx
+++ b/tape_test_xlsx.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>HTS tape results</t>
   </si>
@@ -37,7 +37,7 @@
     <t>n error [+/-]</t>
   </si>
   <si>
-    <t xml:space="preserve">248F-3 </t>
+    <t xml:space="preserve">248F-19 </t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,19 +414,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>20201210081</v>
+        <v>20201027006</v>
       </c>
       <c r="C4">
-        <v>84.07447452698564</v>
+        <v>816.3610747358747</v>
       </c>
       <c r="D4">
-        <v>9.813027077086355</v>
+        <v>419.508702076143</v>
       </c>
       <c r="E4">
-        <v>99.99993900547817</v>
+        <v>2.533678884040108</v>
       </c>
       <c r="F4">
-        <v>258.259466654497</v>
+        <v>0.7066148770379989</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -434,19 +434,39 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>20201210082</v>
+        <v>20201027007</v>
       </c>
       <c r="C5">
-        <v>163.5593349047247</v>
+        <v>171.8897684182772</v>
       </c>
       <c r="D5">
-        <v>68578131.47096683</v>
+        <v>0.06674757216893125</v>
       </c>
       <c r="E5">
-        <v>44.62538704526659</v>
+        <v>40.37504816535063</v>
       </c>
       <c r="F5">
-        <v>30882505.64780365</v>
+        <v>0.6831684792094123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>20201027008</v>
+      </c>
+      <c r="C6">
+        <v>172.8382378878981</v>
+      </c>
+      <c r="D6">
+        <v>0.01968585366899952</v>
+      </c>
+      <c r="E6">
+        <v>31.56235731912708</v>
+      </c>
+      <c r="F6">
+        <v>0.1959617602588581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A few morePr test made, check 20201210
</commit_message>
<xml_diff>
--- a/tape_test_xlsx.xlsx
+++ b/tape_test_xlsx.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>HTS tape results</t>
   </si>
@@ -37,7 +37,7 @@
     <t>n error [+/-]</t>
   </si>
   <si>
-    <t xml:space="preserve">248F-19 </t>
+    <t xml:space="preserve">SOX 717-C 1 </t>
   </si>
 </sst>
 </file>
@@ -378,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -414,19 +414,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>20201027006</v>
+        <v>20201209059</v>
       </c>
       <c r="C4">
-        <v>816.3610747358747</v>
+        <v>159.6991324768351</v>
       </c>
       <c r="D4">
-        <v>419.508702076143</v>
+        <v>0.1049552903810511</v>
       </c>
       <c r="E4">
-        <v>2.533678884040108</v>
+        <v>46.20157618021523</v>
       </c>
       <c r="F4">
-        <v>0.7066148770379989</v>
+        <v>1.462899470367886</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -434,19 +434,19 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>20201027007</v>
+        <v>20201209060</v>
       </c>
       <c r="C5">
-        <v>171.8897684182772</v>
+        <v>159.6154088578845</v>
       </c>
       <c r="D5">
-        <v>0.06674757216893125</v>
+        <v>0.08121870658997199</v>
       </c>
       <c r="E5">
-        <v>40.37504816535063</v>
+        <v>37.48976383711215</v>
       </c>
       <c r="F5">
-        <v>0.6831684792094123</v>
+        <v>0.8996805363756503</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -454,19 +454,79 @@
         <v>7</v>
       </c>
       <c r="B6">
-        <v>20201027008</v>
+        <v>20201209061</v>
       </c>
       <c r="C6">
-        <v>172.8382378878981</v>
+        <v>158.960571292258</v>
       </c>
       <c r="D6">
-        <v>0.01968585366899952</v>
+        <v>0.1339382949238062</v>
       </c>
       <c r="E6">
-        <v>31.56235731912708</v>
+        <v>42.1683928693664</v>
       </c>
       <c r="F6">
-        <v>0.1959617602588581</v>
+        <v>1.489555878658869</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>20201209062</v>
+      </c>
+      <c r="C7">
+        <v>160.0310128606721</v>
+      </c>
+      <c r="D7">
+        <v>0.1143225937587857</v>
+      </c>
+      <c r="E7">
+        <v>32.34361313266743</v>
+      </c>
+      <c r="F7">
+        <v>0.802813239473873</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>20201209063</v>
+      </c>
+      <c r="C8">
+        <v>160.2176175865996</v>
+      </c>
+      <c r="D8">
+        <v>0.08067987777175896</v>
+      </c>
+      <c r="E8">
+        <v>36.82344379992367</v>
+      </c>
+      <c r="F8">
+        <v>0.8276634857217821</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>20201209064</v>
+      </c>
+      <c r="C9">
+        <v>159.9232372688059</v>
+      </c>
+      <c r="D9">
+        <v>0.0793632401463726</v>
+      </c>
+      <c r="E9">
+        <v>37.35252521284222</v>
+      </c>
+      <c r="F9">
+        <v>0.8666815264503328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Peanut butter analysis done
</commit_message>
<xml_diff>
--- a/tape_test_xlsx.xlsx
+++ b/tape_test_xlsx.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>HTS tape results</t>
   </si>
@@ -37,10 +37,7 @@
     <t>n error [+/-]</t>
   </si>
   <si>
-    <t xml:space="preserve">SOJ 803-N2 (2-322) 3,,,,, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOJ 803-N2 (2-322) 3 </t>
+    <t xml:space="preserve">PbSn_4 </t>
   </si>
 </sst>
 </file>
@@ -381,7 +378,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,119 +414,79 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>20201210042</v>
+        <v>20210201033</v>
       </c>
       <c r="C4">
-        <v>180.5427728687814</v>
+        <v>174.4299760564086</v>
       </c>
       <c r="D4">
-        <v>0.06493447368939123</v>
+        <v>0.1882452399594</v>
       </c>
       <c r="E4">
-        <v>38.47173830242762</v>
+        <v>37.84554858073395</v>
       </c>
       <c r="F4">
-        <v>0.7596501519629969</v>
+        <v>1.536449016635741</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>20201210043</v>
+        <v>20210201034</v>
       </c>
       <c r="C5">
-        <v>180.1369443209765</v>
+        <v>175.1892256152058</v>
       </c>
       <c r="D5">
-        <v>0.05103165301648328</v>
+        <v>0.1801372379874642</v>
       </c>
       <c r="E5">
-        <v>38.04397286917502</v>
+        <v>38.64192677454894</v>
       </c>
       <c r="F5">
-        <v>0.6423884147397909</v>
+        <v>1.570378052295473</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>20201210045</v>
+        <v>20210201035</v>
       </c>
       <c r="C6">
-        <v>180.0172184319871</v>
+        <v>175.9431575233957</v>
       </c>
       <c r="D6">
-        <v>0.0515281706184306</v>
+        <v>0.1437538078527957</v>
       </c>
       <c r="E6">
-        <v>38.31522341584989</v>
+        <v>28.00193917968637</v>
       </c>
       <c r="F6">
-        <v>0.6711988811333577</v>
+        <v>0.767042540882385</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>20201210055</v>
+        <v>20210201036</v>
       </c>
       <c r="C7">
-        <v>178.0603918128035</v>
+        <v>175.3689156428129</v>
       </c>
       <c r="D7">
-        <v>0.05821612475474323</v>
+        <v>0.1907870818932693</v>
       </c>
       <c r="E7">
-        <v>32.34054040461744</v>
+        <v>37.06055058813531</v>
       </c>
       <c r="F7">
-        <v>0.5212372278915054</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>20201210056</v>
-      </c>
-      <c r="C8">
-        <v>177.7254317404144</v>
-      </c>
-      <c r="D8">
-        <v>0.05034451334953678</v>
-      </c>
-      <c r="E8">
-        <v>38.84520308990845</v>
-      </c>
-      <c r="F8">
-        <v>0.6843883330943414</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>20201210057</v>
-      </c>
-      <c r="C9">
-        <v>177.9056332511805</v>
-      </c>
-      <c r="D9">
-        <v>0.04543551620043342</v>
-      </c>
-      <c r="E9">
-        <v>30.85645599536549</v>
-      </c>
-      <c r="F9">
-        <v>0.4596106340641563</v>
+        <v>1.569102528353512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>